<commit_message>
Add parse main thread func
</commit_message>
<xml_diff>
--- a/log-parsed.xlsx
+++ b/log-parsed.xlsx
@@ -324,9 +324,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1"/>
-    <row r="2">
-      <c r="A2" t="str">
+    <row r="1">
+      <c r="A1" t="str">
         <v>Hello world.</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Create main thread table
</commit_message>
<xml_diff>
--- a/log-parsed.xlsx
+++ b/log-parsed.xlsx
@@ -326,8 +326,116 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>Hello world.</v>
-      </c>
+        <v>主线程开始</v>
+      </c>
+      <c r="B1" t="str"/>
+      <c r="C1" t="str">
+        <v>2019-08-07 15:36:04.947</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>basicOpe</v>
+      </c>
+      <c r="B2" t="str">
+        <v>37</v>
+      </c>
+      <c r="C2" t="str">
+        <v>2019-08-07 15:36:04.998</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>basicProd</v>
+      </c>
+      <c r="B3" t="str">
+        <v>3</v>
+      </c>
+      <c r="C3" t="str">
+        <v>2019-08-07 15:36:05.001</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>basicOwnTime</v>
+      </c>
+      <c r="B4" t="str">
+        <v>15</v>
+      </c>
+      <c r="C4" t="str">
+        <v>2019-08-07 15:36:05.016</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>rpushTime</v>
+      </c>
+      <c r="B5" t="str">
+        <v>3</v>
+      </c>
+      <c r="C5" t="str">
+        <v>2019-08-07 15:36:05.019</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>zaddTime</v>
+      </c>
+      <c r="B6" t="str">
+        <v>1</v>
+      </c>
+      <c r="C6" t="str">
+        <v>2019-08-07 15:36:05.020</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>matchedRuleTime</v>
+      </c>
+      <c r="B7" t="str">
+        <v>158</v>
+      </c>
+      <c r="C7" t="str">
+        <v>2019-08-07 15:36:05.178</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>zaddHistory</v>
+      </c>
+      <c r="B8" t="str">
+        <v>166</v>
+      </c>
+      <c r="C8" t="str">
+        <v>2019-08-07 15:36:05.344</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>主线程调用子线程(MAIN CALL SUB)</v>
+      </c>
+      <c r="B9" t="str"/>
+      <c r="C9" t="str">
+        <v>2019-08-07 15:36:05.496</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>回主线程 (MAIN RETURN)</v>
+      </c>
+      <c r="B10" t="str"/>
+      <c r="C10" t="str">
+        <v>2019-08-07 15:36:09.602</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>总时间</v>
+      </c>
+      <c r="B11" t="str">
+        <v>4106</v>
+      </c>
+      <c r="C11" t="str"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>